<commit_message>
Upload June 15, 2023
</commit_message>
<xml_diff>
--- a/student-dms.xlsx
+++ b/student-dms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Student\2302.E1\github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EECA0E-1115-487A-8096-86EA1F5BD54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5851799A-9819-47FD-A6C3-9F607AAF1215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1055" yWindow="1055" windowWidth="17705" windowHeight="9405" xr2:uid="{C213B660-CC71-4CF0-9CDC-E7441964446C}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="17705" windowHeight="9405" xr2:uid="{C213B660-CC71-4CF0-9CDC-E7441964446C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -314,25 +314,40 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -651,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293C4592-611C-4D00-BD7D-58519D2BB220}">
   <dimension ref="B4:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -663,242 +678,242 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B4" s="6">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B5" s="6"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B6" s="6"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B7" s="6">
+      <c r="B7" s="9">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B8" s="6"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B9" s="6"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B10" s="6">
+      <c r="B10" s="9">
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B11" s="6"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B12" s="6"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B13" s="6">
+      <c r="B13" s="9">
         <v>4</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B14" s="6"/>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B15" s="6"/>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B16" s="6">
+      <c r="B16" s="9">
         <v>5</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B17" s="6"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B18" s="6"/>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B19" s="6">
+      <c r="B19" s="9">
         <v>6</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B20" s="6"/>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B21" s="6"/>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B22" s="6">
+      <c r="B22" s="9">
         <v>7</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B23" s="6"/>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.75">
-      <c r="B24" s="6"/>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>